<commit_message>
Update IP - EX 20 - Funcao Somase e Somases (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 20 - Funcao Somase e Somases (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 20 - Funcao Somase e Somases (Anexo).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B12AA41-A7AC-4E20-B4A6-460217C8AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BFF250-057F-444F-9410-5A88702EF609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
     <sheet name="EXPLICAÇÃO" sheetId="10" r:id="rId2"/>
     <sheet name="EXERCICIO 1" sheetId="15" r:id="rId3"/>
+    <sheet name="BD Lista" sheetId="16" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="anscount" hidden="1">2</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="52">
   <si>
     <t>FUNÇÃO SOMASE</t>
   </si>
@@ -226,7 +227,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,13 +358,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="28"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
@@ -411,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1086,6 +1080,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="dotted">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1096,7 +1155,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1249,40 +1308,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="5" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="5" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="5" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,58 +1365,65 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="17" fillId="5" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1915,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2104,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I85" sqref="I85"/>
+    <sheetView showGridLines="0" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,9 +2269,11 @@
       <c r="E8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="66"/>
+      <c r="F8" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="84"/>
+      <c r="H8" s="85"/>
       <c r="J8" t="s">
         <v>48</v>
       </c>
@@ -2241,9 +2291,12 @@
       <c r="E10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="F10" s="86">
+        <f>SUMIF($B$11:$B$40,F8,$C$11:$C$40)</f>
+        <v>372</v>
+      </c>
+      <c r="G10" s="87"/>
+      <c r="H10" s="88"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="33" t="s">
@@ -2490,9 +2543,11 @@
       <c r="G42" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="64"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="66"/>
+      <c r="H42" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="I42" s="84"/>
+      <c r="J42" s="85"/>
     </row>
     <row r="43" spans="2:10" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G43" s="25"/>
@@ -2501,9 +2556,11 @@
       <c r="G44" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="64"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="66"/>
+      <c r="H44" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="84"/>
+      <c r="J44" s="85"/>
     </row>
     <row r="45" spans="2:10" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G45" s="25"/>
@@ -2515,9 +2572,12 @@
       <c r="G46" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H46" s="67"/>
-      <c r="I46" s="68"/>
-      <c r="J46" s="69"/>
+      <c r="H46" s="86">
+        <f>SUMIFS($D$49:$D$78,$B$49:$B$78,$H$42,$C$49:$C$78,$H$44)</f>
+        <v>154</v>
+      </c>
+      <c r="I46" s="87"/>
+      <c r="J46" s="88"/>
     </row>
     <row r="47" spans="2:10" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H47" s="1"/>
@@ -2869,10 +2929,10 @@
       <c r="H79" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I79" s="76">
+      <c r="I79" s="70">
         <v>42014</v>
       </c>
-      <c r="J79" s="77"/>
+      <c r="J79" s="71"/>
     </row>
     <row r="80" spans="2:10" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H80" s="25"/>
@@ -2883,10 +2943,10 @@
       <c r="H81" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="I81" s="76">
+      <c r="I81" s="70">
         <v>42017</v>
       </c>
-      <c r="J81" s="77"/>
+      <c r="J81" s="71"/>
     </row>
     <row r="82" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="26" t="s">
@@ -2913,8 +2973,11 @@
       <c r="H84" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I84" s="78"/>
-      <c r="J84" s="79"/>
+      <c r="I84" s="72">
+        <f>SUMIFS(E85:E92,$D$85:$D$92,"&gt;=" &amp; I79,$D$85:$D$92,"&lt;=" &amp; I81)</f>
+        <v>268</v>
+      </c>
+      <c r="J84" s="73"/>
     </row>
     <row r="85" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="48" t="s">
@@ -2999,11 +3062,11 @@
       <c r="E90" s="30">
         <v>44</v>
       </c>
-      <c r="H90" s="80" t="s">
+      <c r="H90" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="I90" s="81"/>
-      <c r="J90" s="82"/>
+      <c r="I90" s="75"/>
+      <c r="J90" s="76"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91" s="29" t="s">
@@ -3018,9 +3081,9 @@
       <c r="E91" s="30">
         <v>168</v>
       </c>
-      <c r="H91" s="83"/>
-      <c r="I91" s="84"/>
-      <c r="J91" s="85"/>
+      <c r="H91" s="77"/>
+      <c r="I91" s="78"/>
+      <c r="J91" s="79"/>
     </row>
     <row r="92" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="31" t="s">
@@ -3035,38 +3098,56 @@
       <c r="E92" s="32">
         <v>158</v>
       </c>
-      <c r="H92" s="86"/>
-      <c r="I92" s="87"/>
-      <c r="J92" s="88"/>
+      <c r="H92" s="80"/>
+      <c r="I92" s="81"/>
+      <c r="J92" s="82"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H93" s="70" t="s">
+      <c r="H93" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="I93" s="71"/>
-      <c r="J93" s="72"/>
+      <c r="I93" s="65"/>
+      <c r="J93" s="66"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H94" s="73"/>
-      <c r="I94" s="74"/>
-      <c r="J94" s="75"/>
+      <c r="H94" s="67"/>
+      <c r="I94" s="68"/>
+      <c r="J94" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H93:J94"/>
-    <mergeCell ref="I79:J79"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="H90:J92"/>
     <mergeCell ref="B2:Q6"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="H42:J42"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H93:J94"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="H90:J92"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C491AA6-2368-4D47-B176-198610CDF9AC}">
+          <x14:formula1>
+            <xm:f>'BD Lista'!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8:H8 H42:J42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A1DB4C0D-A1D7-43F8-A202-CC1F0E4AFE48}">
+          <x14:formula1>
+            <xm:f>'BD Lista'!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>H44:J44</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3074,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:P502"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32:O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,7 +3228,9 @@
       <c r="I4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="37"/>
+      <c r="J4" s="37">
+        <v>1</v>
+      </c>
       <c r="L4" s="54" t="s">
         <v>34</v>
       </c>
@@ -3168,10 +3251,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="I5" s="24"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="100"/>
+      <c r="L5" s="95">
+        <f>SUMIFS($E$3:$E$502,$B$3:$B$502,"&gt;="&amp;$J$4,B3:B502,"&lt;="&amp;$J$6)</f>
+        <v>8897</v>
+      </c>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="97"/>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -3191,11 +3277,13 @@
       <c r="I6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="103"/>
+      <c r="J6" s="37">
+        <v>11</v>
+      </c>
+      <c r="L6" s="98"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="100"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -3213,10 +3301,10 @@
       </c>
       <c r="G7" s="4"/>
       <c r="I7" s="24"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
-      <c r="O7" s="106"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="103"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -3332,13 +3420,15 @@
       <c r="I13" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="37"/>
+      <c r="J13" s="37" t="s">
+        <v>26</v>
+      </c>
       <c r="L13" s="54" t="s">
         <v>34</v>
       </c>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="29">
         <v>12</v>
       </c>
@@ -3352,13 +3442,16 @@
         <v>390</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="91"/>
+      <c r="L14" s="95">
+        <f>SUMIF($C$3:$C$502,J13,E3:E502)</f>
+        <v>75899</v>
+      </c>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="97"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="29">
         <v>13</v>
       </c>
@@ -3372,13 +3465,13 @@
         <v>526</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="94"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="100"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="29">
         <v>14</v>
       </c>
@@ -3392,10 +3485,10 @@
         <v>868</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="96"/>
-      <c r="O16" s="97"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="103"/>
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
@@ -3512,13 +3605,15 @@
       <c r="I22" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="37"/>
+      <c r="J22" s="37" t="s">
+        <v>7</v>
+      </c>
       <c r="L22" s="54" t="s">
         <v>34</v>
       </c>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="29">
         <v>21</v>
       </c>
@@ -3532,13 +3627,16 @@
         <v>1131</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="L23" s="89"/>
-      <c r="M23" s="90"/>
-      <c r="N23" s="90"/>
-      <c r="O23" s="91"/>
+      <c r="L23" s="95">
+        <f>SUMIF($D:$D,$J$22,E:E)</f>
+        <v>50426</v>
+      </c>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="97"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="29">
         <v>22</v>
       </c>
@@ -3552,13 +3650,13 @@
         <v>644</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="93"/>
-      <c r="O24" s="94"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="100"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="29">
         <v>23</v>
       </c>
@@ -3572,10 +3670,10 @@
         <v>709</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="96"/>
-      <c r="N25" s="96"/>
-      <c r="O25" s="97"/>
+      <c r="L25" s="101"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="103"/>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
@@ -3691,13 +3789,15 @@
       <c r="I31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="37"/>
+      <c r="J31" s="37" t="s">
+        <v>26</v>
+      </c>
       <c r="L31" s="54" t="s">
         <v>34</v>
       </c>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="29">
         <v>30</v>
       </c>
@@ -3712,13 +3812,16 @@
       </c>
       <c r="G32" s="4"/>
       <c r="I32" s="24"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="90"/>
-      <c r="O32" s="91"/>
+      <c r="L32" s="95">
+        <f>SUMIFS($E:$E,$C:$C,$J$31,$D:$D,$J$33)</f>
+        <v>10994</v>
+      </c>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="97"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="29">
         <v>31</v>
       </c>
@@ -3735,14 +3838,16 @@
       <c r="I33" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="37"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="94"/>
+      <c r="J33" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="98"/>
+      <c r="M33" s="99"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="100"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="29">
         <v>32</v>
       </c>
@@ -3756,10 +3861,10 @@
         <v>1030</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="96"/>
-      <c r="N34" s="96"/>
-      <c r="O34" s="97"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="103"/>
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -10334,5 +10439,2645 @@
     <mergeCell ref="L23:O25"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{072D07AA-8B4A-4366-9E63-3BEEE4C22CA6}">
+          <x14:formula1>
+            <xm:f>'BD Lista'!$C$2:$C$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>J4 J6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{692CB4F0-2855-4B00-886D-6A2F0596E34E}">
+          <x14:formula1>
+            <xm:f>'BD Lista'!$D$2:$D$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>J13 J31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C89EF2-AAF7-48CE-B7CD-A9CEE26D0D70}">
+          <x14:formula1>
+            <xm:f>'BD Lista'!$E$2:$E$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>J22 J33</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D647BCEE-D375-4891-A110-C6EAFE5FD68F}">
+  <dimension ref="A1:E501"/>
+  <sheetViews>
+    <sheetView topLeftCell="A1048523" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="94" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="92">
+        <v>1</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="92">
+        <v>2</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="92">
+        <v>3</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="92">
+        <v>4</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="92">
+        <v>5</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="92">
+        <v>6</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="92">
+        <v>7</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="92">
+        <v>8</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="92">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="92">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="92">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="92">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="92">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="92">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="92">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="92">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="92">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="92">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="92">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="92">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="92">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="92">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="92">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="92">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="92">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="92">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="92">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="92">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="92">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="92">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="92">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="92">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="92">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="92">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="92">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="92">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="92">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="92">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="92">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="92">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="92">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="92">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="92">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="92">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="92">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="92">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="92">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="92">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="92">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="92">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="92">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="92">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="92">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="92">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="92">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="92">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="92">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="92">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="92">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="92">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="92">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="92">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="92">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="92">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="92">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="92">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="92">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="92">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="92">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="92">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="92">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="92">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="92">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="92">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="92">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="92">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="92">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="92">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="92">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="92">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="92">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="92">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="92">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="92">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="92">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="92">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="92">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="92">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="92">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="92">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="92">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="92">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="92">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="92">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="92">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="92">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="92">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="92">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="92">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="92">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="92">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="92">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="92">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="92">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="92">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="92">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="92">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="92">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="92">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="92">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="92">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="92">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="92">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="92">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="92">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="92">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="92">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="92">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="92">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="92">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="92">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="92">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="92">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="92">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="92">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="92">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="92">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="92">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="92">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="92">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="92">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="92">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="92">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="92">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="92">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="92">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="92">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="92">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="92">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="92">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="92">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="92">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="92">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="92">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="92">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="92">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="92">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="92">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="92">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="92">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="92">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="92">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="92">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="92">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="92">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="92">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="92">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="92">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="92">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="92">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="92">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="92">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="92">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="92">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="92">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="92">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="92">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="92">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="92">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="92">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="92">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="92">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="92">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="92">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="92">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="92">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="92">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="92">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="92">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="92">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="92">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C189" s="92">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="92">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C191" s="92">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C192" s="92">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C193" s="92">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C194" s="92">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C195" s="92">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C196" s="92">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C197" s="92">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C198" s="92">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C199" s="92">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C200" s="92">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C201" s="92">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C202" s="92">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C203" s="92">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C204" s="92">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C205" s="92">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C206" s="92">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C207" s="92">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C208" s="92">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C209" s="92">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C210" s="92">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="92">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C212" s="92">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C213" s="92">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C214" s="92">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C215" s="92">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C216" s="92">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C217" s="92">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C218" s="92">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C219" s="92">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C220" s="92">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C221" s="92">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C222" s="92">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C223" s="92">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C224" s="92">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" s="92">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C226" s="92">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C227" s="92">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C228" s="92">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C229" s="92">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C230" s="92">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C231" s="92">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C232" s="92">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C233" s="92">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C234" s="92">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C235" s="92">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C236" s="92">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C237" s="92">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C238" s="92">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C239" s="92">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C240" s="92">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C241" s="92">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C242" s="92">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C243" s="92">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C244" s="92">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C245" s="92">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C246" s="92">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C247" s="92">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C248" s="92">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C249" s="92">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C250" s="92">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C251" s="92">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C252" s="92">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C253" s="92">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C254" s="92">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C255" s="92">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C256" s="92">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C257" s="92">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C258" s="92">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C259" s="92">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C260" s="92">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C261" s="92">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C262" s="92">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C263" s="92">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C264" s="92">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C265" s="92">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C266" s="92">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C267" s="92">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C268" s="92">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C269" s="92">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C270" s="92">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C271" s="92">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C272" s="92">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C273" s="92">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C274" s="92">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C275" s="92">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C276" s="92">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C277" s="92">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C278" s="92">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C279" s="92">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C280" s="92">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C281" s="92">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C282" s="92">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C283" s="92">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C284" s="92">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C285" s="92">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C286" s="92">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C287" s="92">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C288" s="92">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C289" s="92">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C290" s="92">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C291" s="92">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C292" s="92">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C293" s="92">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C294" s="92">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C295" s="92">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C296" s="92">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C297" s="92">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C298" s="92">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C299" s="92">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C300" s="92">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C301" s="92">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C302" s="92">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C303" s="92">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C304" s="92">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C305" s="92">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C306" s="92">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C307" s="92">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C308" s="92">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C309" s="92">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C310" s="92">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C311" s="92">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C312" s="92">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C313" s="92">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C314" s="92">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C315" s="92">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C316" s="92">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C317" s="92">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C318" s="92">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C319" s="92">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C320" s="92">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C321" s="92">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C322" s="92">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C323" s="92">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C324" s="92">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C325" s="92">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C326" s="92">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C327" s="92">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C328" s="92">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C329" s="92">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C330" s="92">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C331" s="92">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C332" s="92">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C333" s="92">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C334" s="92">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C335" s="92">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C336" s="92">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C337" s="92">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C338" s="92">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C339" s="92">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C340" s="92">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C341" s="92">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C342" s="92">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C343" s="92">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C344" s="92">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C345" s="92">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C346" s="92">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C347" s="92">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C348" s="92">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C349" s="92">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C350" s="92">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C351" s="92">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C352" s="92">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C353" s="92">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C354" s="92">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C355" s="92">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C356" s="92">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C357" s="92">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C358" s="92">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C359" s="92">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C360" s="92">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C361" s="92">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C362" s="92">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="363" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C363" s="92">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C364" s="92">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C365" s="92">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="366" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C366" s="92">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="367" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C367" s="92">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="368" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C368" s="92">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C369" s="92">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C370" s="92">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C371" s="92">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C372" s="92">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C373" s="92">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="374" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C374" s="92">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="375" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C375" s="92">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="376" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C376" s="92">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="377" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C377" s="92">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C378" s="92">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="379" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C379" s="92">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="380" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C380" s="92">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="381" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C381" s="92">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="382" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C382" s="92">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="383" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C383" s="92">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="384" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C384" s="92">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="385" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C385" s="92">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="386" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C386" s="92">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="387" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C387" s="92">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="388" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C388" s="92">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="389" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C389" s="92">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="390" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C390" s="92">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="391" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C391" s="92">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="392" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C392" s="92">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="393" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C393" s="92">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="394" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C394" s="92">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C395" s="92">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="396" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C396" s="92">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="397" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C397" s="92">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="398" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C398" s="92">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="399" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C399" s="92">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="400" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C400" s="92">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="401" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C401" s="92">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="402" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C402" s="92">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="403" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C403" s="92">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="404" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C404" s="92">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C405" s="92">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C406" s="92">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C407" s="92">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C408" s="92">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C409" s="92">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C410" s="92">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C411" s="92">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C412" s="92">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C413" s="92">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C414" s="92">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C415" s="92">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C416" s="92">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C417" s="92">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="418" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C418" s="92">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="419" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C419" s="92">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C420" s="92">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C421" s="92">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C422" s="92">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C423" s="92">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C424" s="92">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C425" s="92">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="426" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C426" s="92">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C427" s="92">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C428" s="92">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C429" s="92">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="430" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C430" s="92">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="431" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C431" s="92">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="432" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C432" s="92">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="433" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C433" s="92">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="434" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C434" s="92">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="435" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C435" s="92">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="436" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C436" s="92">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="437" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C437" s="92">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="438" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C438" s="92">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="439" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C439" s="92">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="440" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C440" s="92">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="441" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C441" s="92">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="442" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C442" s="92">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="443" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C443" s="92">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="444" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C444" s="92">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="445" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C445" s="92">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="446" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C446" s="92">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="447" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C447" s="92">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="448" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C448" s="92">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="449" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C449" s="92">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="450" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C450" s="92">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="451" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C451" s="92">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="452" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C452" s="92">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="453" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C453" s="92">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="454" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C454" s="92">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="455" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C455" s="92">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="456" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C456" s="92">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="457" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C457" s="92">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="458" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C458" s="92">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="459" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C459" s="92">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C460" s="92">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="461" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C461" s="92">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C462" s="92">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="463" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C463" s="92">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="464" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C464" s="92">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="465" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C465" s="92">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="466" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C466" s="92">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="467" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C467" s="92">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="468" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C468" s="92">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="469" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C469" s="92">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="470" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C470" s="92">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="471" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C471" s="92">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="472" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C472" s="92">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="473" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C473" s="92">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="474" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C474" s="92">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="475" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C475" s="92">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="476" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C476" s="92">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="477" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C477" s="92">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="478" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C478" s="92">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="479" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C479" s="92">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="480" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C480" s="92">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="481" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C481" s="92">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="482" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C482" s="92">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="483" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C483" s="92">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="484" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C484" s="92">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="485" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C485" s="92">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="486" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C486" s="92">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="487" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C487" s="92">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="488" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C488" s="92">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="489" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C489" s="92">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="490" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C490" s="92">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="491" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C491" s="92">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C492" s="92">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="493" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C493" s="92">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="494" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C494" s="92">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="495" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C495" s="92">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="496" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C496" s="92">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C497" s="92">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="498" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C498" s="92">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="499" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C499" s="92">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="500" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C500" s="92">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="501" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C501" s="93">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>